<commit_message>
New 'seen' variable added
</commit_message>
<xml_diff>
--- a/zombies.xlsx
+++ b/zombies.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GonzaloGGC/Desktop/code/zombies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C5FF9-543C-9540-99D0-41BE8ED50999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{753FE9C6-5B25-554F-80E2-774441457194}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{1CE32F32-CAC9-BF49-AB2E-69AF6A7F113F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="zombies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -17085,7 +17085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F468E6-A17C-E246-A3FD-AB15D793798B}">
   <dimension ref="A1:F1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A988" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>

</xml_diff>